<commit_message>
Made the script automatically give water to the plants.
</commit_message>
<xml_diff>
--- a/device/motorCalibration.xlsx
+++ b/device/motorCalibration.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Library/WebServer/Documents/git/AutoHomeProjects/ELumenHub/device/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A7ED7E-EB81-D840-9298-8D988FC0B2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DA6D4C-FA47-AB4F-920D-F74AD993088E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{DF02C44D-7449-1B43-9351-587A6E88EB55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Plant</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>mL/s</t>
+  </si>
+  <si>
+    <t>offset</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>ms/mL</t>
   </si>
 </sst>
 </file>
@@ -3590,10 +3599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B269BF2-DD9E-904D-97B7-5A1CBEF94229}">
-  <dimension ref="A3:P27"/>
+  <dimension ref="A3:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3781,7 +3790,7 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <f t="shared" ref="N5:N24" si="0">IF(F12&lt;&gt;0,F12,"")</f>
+        <f t="shared" ref="N12:N23" si="0">IF(F12&lt;&gt;0,F12,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -3802,7 +3811,7 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <f t="shared" ref="M6:M24" si="1">IF(E13&lt;&gt;0,E13,"")</f>
+        <f t="shared" ref="M13:M23" si="1">IF(E13&lt;&gt;0,E13,"")</f>
         <v>1</v>
       </c>
       <c r="N13">
@@ -3871,7 +3880,7 @@
         <v>0.5</v>
       </c>
       <c r="O16">
-        <f t="shared" ref="O5:O24" si="2">IF(G16&lt;&gt;0,G16,"")</f>
+        <f t="shared" ref="O16:O24" si="2">IF(G16&lt;&gt;0,G16,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -3912,7 +3921,7 @@
         <v>1</v>
       </c>
       <c r="P18">
-        <f t="shared" ref="P5:P24" si="3">IF(H18&lt;&gt;0,H18,"")</f>
+        <f t="shared" ref="P18:P24" si="3">IF(H18&lt;&gt;0,H18,"")</f>
         <v>1</v>
       </c>
     </row>
@@ -4072,6 +4081,27 @@
         <v>12.5</v>
       </c>
     </row>
+    <row r="25" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="L25" t="s">
+        <v>8</v>
+      </c>
+      <c r="M25">
+        <f>INTERCEPT(M5:M24,$D$5:$D$24)</f>
+        <v>-1.1759202920596294</v>
+      </c>
+      <c r="N25">
+        <f t="shared" ref="N25:P25" si="4">INTERCEPT(N5:N24,$D$5:$D$24)</f>
+        <v>-0.75257544224765827</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="4"/>
+        <v>-1.5298495602194544</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="4"/>
+        <v>-1.5484083742928689</v>
+      </c>
+    </row>
     <row r="26" spans="4:16" x14ac:dyDescent="0.2">
       <c r="L26" t="s">
         <v>4</v>
@@ -4081,15 +4111,15 @@
         <v>1.6368775986208297E-3</v>
       </c>
       <c r="N26">
-        <f t="shared" ref="N26:P26" si="4">SLOPE(N5:N24,$D$5:$D$24)</f>
+        <f t="shared" ref="N26:P26" si="5">SLOPE(N5:N24,$D$5:$D$24)</f>
         <v>1.3731356226153312E-3</v>
       </c>
       <c r="O26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0023839588957589E-3</v>
       </c>
       <c r="P26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.1517898544004456E-4</v>
       </c>
     </row>
@@ -4102,20 +4132,63 @@
         <v>26.83405899378409</v>
       </c>
       <c r="N27">
-        <f t="shared" ref="N27:P27" si="5">N26*$A$4*1000</f>
+        <f t="shared" ref="N27:P27" si="6">N26*$A$4*1000</f>
         <v>22.51042004287428</v>
       </c>
       <c r="O27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>16.432523916323916</v>
       </c>
       <c r="P27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>15.002934187541712</v>
+      </c>
+    </row>
+    <row r="28" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="L28" t="s">
+        <v>7</v>
+      </c>
+      <c r="M28">
+        <f>-M25/M26</f>
+        <v>718.39231781925218</v>
+      </c>
+      <c r="N28">
+        <f t="shared" ref="N28:P28" si="7">-N25/N26</f>
+        <v>548.07072939690534</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="7"/>
+        <v>1526.2111356059204</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="7"/>
+        <v>1691.9186289536024</v>
+      </c>
+    </row>
+    <row r="29" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="L29" t="s">
+        <v>9</v>
+      </c>
+      <c r="M29">
+        <f>1000/M27</f>
+        <v>37.266072949740575</v>
+      </c>
+      <c r="N29">
+        <f t="shared" ref="N29:P29" si="8">1000/N27</f>
+        <v>44.423871171455644</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="8"/>
+        <v>60.854924361717153</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="8"/>
+        <v>66.653628383599127</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>